<commit_message>
believe I've identified all bad zombies
</commit_message>
<xml_diff>
--- a/data/zombie2.xlsx
+++ b/data/zombie2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,142 +366,137 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>51</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>69</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>81</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>143</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>145</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>160</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>223</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>239</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>277</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>307</v>
+        <v>513</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>324</v>
+        <v>529</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>353</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>513</v>
+        <v>765</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>529</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>568</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>765</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1216</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1222</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>1228</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1234</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1325</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1332</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1455</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1533</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>1357</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>